<commit_message>
refactored directory structure and added validation logic for data
</commit_message>
<xml_diff>
--- a/oe_production_2new .xlsx
+++ b/oe_production_2new .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eperiyasamy/oe-reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2034CB2-8DFD-804B-A7E7-22A2FC037361}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFF941D-3E1D-0E4A-B2CB-6CEEBE0E8526}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="93">
   <si>
     <t>machine_id</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>drum_mpm</t>
+  </si>
+  <si>
+    <t>row id</t>
   </si>
 </sst>
 </file>
@@ -791,2285 +794,2293 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:HX15"/>
+  <dimension ref="A1:HY15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HL1" workbookViewId="0">
-      <selection activeCell="CH11" sqref="CH11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="5.5" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="10" width="11.83203125" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" customWidth="1"/>
-    <col min="12" max="12" width="6" style="3" customWidth="1"/>
-    <col min="13" max="13" width="14" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="15" max="15" width="8" style="3" customWidth="1"/>
-    <col min="16" max="17" width="7.83203125" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" customWidth="1"/>
-    <col min="20" max="20" width="12.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" customWidth="1"/>
-    <col min="23" max="23" width="11.1640625" customWidth="1"/>
-    <col min="24" max="24" width="9.5" customWidth="1"/>
-    <col min="25" max="25" width="13.83203125" customWidth="1"/>
-    <col min="26" max="26" width="8.83203125" style="5"/>
-    <col min="28" max="28" width="6.83203125" customWidth="1"/>
-    <col min="29" max="29" width="10.83203125" customWidth="1"/>
-    <col min="30" max="30" width="13.83203125" customWidth="1"/>
-    <col min="32" max="34" width="11.5" customWidth="1"/>
-    <col min="37" max="38" width="13.6640625" customWidth="1"/>
-    <col min="41" max="41" width="12.1640625" customWidth="1"/>
-    <col min="42" max="42" width="11.1640625" customWidth="1"/>
-    <col min="43" max="43" width="12.1640625" customWidth="1"/>
-    <col min="45" max="45" width="5.6640625" style="19" customWidth="1"/>
-    <col min="47" max="47" width="6.5" customWidth="1"/>
-    <col min="48" max="48" width="10.83203125" customWidth="1"/>
-    <col min="49" max="49" width="13.83203125" customWidth="1"/>
-    <col min="50" max="50" width="11.83203125" customWidth="1"/>
-    <col min="51" max="53" width="11.5" customWidth="1"/>
-    <col min="54" max="54" width="13.5" customWidth="1"/>
-    <col min="55" max="55" width="11.1640625" customWidth="1"/>
-    <col min="56" max="56" width="10" customWidth="1"/>
-    <col min="57" max="57" width="9.33203125" customWidth="1"/>
-    <col min="60" max="60" width="12.5" customWidth="1"/>
-    <col min="61" max="61" width="10.83203125" customWidth="1"/>
-    <col min="62" max="62" width="12.83203125" customWidth="1"/>
-    <col min="63" max="63" width="4.33203125" style="19" customWidth="1"/>
-    <col min="65" max="65" width="6.1640625" customWidth="1"/>
-    <col min="66" max="66" width="10.83203125" customWidth="1"/>
-    <col min="67" max="67" width="12" customWidth="1"/>
-    <col min="68" max="68" width="8.83203125" customWidth="1"/>
-    <col min="69" max="71" width="11.5" customWidth="1"/>
-    <col min="72" max="72" width="12.33203125" customWidth="1"/>
-    <col min="73" max="73" width="9.1640625" customWidth="1"/>
-    <col min="74" max="74" width="7.33203125" customWidth="1"/>
-    <col min="75" max="75" width="7.83203125" customWidth="1"/>
-    <col min="76" max="76" width="7.5" customWidth="1"/>
-    <col min="77" max="77" width="12.5" customWidth="1"/>
-    <col min="78" max="78" width="10.83203125" customWidth="1"/>
-    <col min="79" max="79" width="11.5" customWidth="1"/>
-    <col min="80" max="80" width="4.5" style="19" customWidth="1"/>
-    <col min="82" max="82" width="5.1640625" customWidth="1"/>
-    <col min="83" max="83" width="13.33203125" customWidth="1"/>
-    <col min="84" max="84" width="12.83203125" customWidth="1"/>
-    <col min="85" max="85" width="10.5" customWidth="1"/>
-    <col min="86" max="88" width="11.33203125" customWidth="1"/>
-    <col min="89" max="89" width="9" customWidth="1"/>
-    <col min="90" max="91" width="13.33203125" customWidth="1"/>
-    <col min="92" max="92" width="9.1640625" customWidth="1"/>
-    <col min="93" max="93" width="7" customWidth="1"/>
-    <col min="96" max="96" width="12.83203125" customWidth="1"/>
-    <col min="97" max="97" width="6.6640625" style="3" customWidth="1"/>
-    <col min="98" max="98" width="12.83203125" customWidth="1"/>
-    <col min="99" max="99" width="10.1640625" customWidth="1"/>
-    <col min="100" max="100" width="11.1640625" customWidth="1"/>
-    <col min="101" max="101" width="12.1640625" customWidth="1"/>
-    <col min="102" max="102" width="3.33203125" customWidth="1"/>
-    <col min="104" max="104" width="7.5" customWidth="1"/>
-    <col min="105" max="105" width="9.6640625" customWidth="1"/>
-    <col min="106" max="106" width="12.1640625" customWidth="1"/>
-    <col min="107" max="107" width="12.33203125" customWidth="1"/>
-    <col min="108" max="110" width="12.1640625" customWidth="1"/>
-    <col min="111" max="111" width="9.1640625" customWidth="1"/>
-    <col min="112" max="113" width="13.33203125" customWidth="1"/>
-    <col min="114" max="114" width="9.1640625" customWidth="1"/>
-    <col min="115" max="115" width="6" customWidth="1"/>
-    <col min="116" max="116" width="7.6640625" customWidth="1"/>
-    <col min="117" max="117" width="7.5" customWidth="1"/>
-    <col min="118" max="118" width="12.83203125" customWidth="1"/>
-    <col min="119" max="119" width="6.6640625" style="3" customWidth="1"/>
-    <col min="120" max="120" width="11.5" customWidth="1"/>
-    <col min="121" max="121" width="10.33203125" customWidth="1"/>
-    <col min="122" max="122" width="13.1640625" customWidth="1"/>
-    <col min="123" max="123" width="12.1640625" customWidth="1"/>
-    <col min="124" max="124" width="4.6640625" style="14" customWidth="1"/>
-    <col min="128" max="128" width="7.5" customWidth="1"/>
-    <col min="129" max="129" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="12.1640625" customWidth="1"/>
-    <col min="132" max="132" width="12.33203125" customWidth="1"/>
-    <col min="133" max="133" width="13.33203125" customWidth="1"/>
-    <col min="134" max="134" width="12.5" customWidth="1"/>
-    <col min="135" max="135" width="10.33203125" customWidth="1"/>
-    <col min="136" max="136" width="6" style="3" customWidth="1"/>
-    <col min="137" max="138" width="13.33203125" customWidth="1"/>
-    <col min="139" max="139" width="7.1640625" style="3" customWidth="1"/>
-    <col min="140" max="141" width="7.83203125" customWidth="1"/>
-    <col min="142" max="142" width="12.1640625" style="3" customWidth="1"/>
-    <col min="143" max="143" width="10.6640625" customWidth="1"/>
-    <col min="144" max="144" width="12.1640625" customWidth="1"/>
-    <col min="145" max="145" width="11" customWidth="1"/>
-    <col min="146" max="146" width="13.1640625" customWidth="1"/>
-    <col min="147" max="147" width="10.83203125" customWidth="1"/>
-    <col min="148" max="148" width="9.83203125" customWidth="1"/>
-    <col min="149" max="149" width="13.1640625" customWidth="1"/>
-    <col min="150" max="150" width="3.83203125" style="14" customWidth="1"/>
-    <col min="154" max="154" width="12.5" customWidth="1"/>
-    <col min="156" max="158" width="11.33203125" customWidth="1"/>
-    <col min="159" max="159" width="9.1640625" customWidth="1"/>
-    <col min="160" max="160" width="6.5" customWidth="1"/>
-    <col min="161" max="162" width="12.83203125" customWidth="1"/>
-    <col min="164" max="164" width="9.1640625" customWidth="1"/>
-    <col min="165" max="165" width="12.1640625" customWidth="1"/>
-    <col min="166" max="166" width="12.83203125" customWidth="1"/>
-    <col min="167" max="167" width="14.1640625" customWidth="1"/>
-    <col min="169" max="169" width="3.6640625" style="15" customWidth="1"/>
-    <col min="171" max="171" width="10" customWidth="1"/>
-    <col min="173" max="173" width="7.5" customWidth="1"/>
-    <col min="174" max="174" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="11.33203125" customWidth="1"/>
-    <col min="177" max="177" width="11.1640625" customWidth="1"/>
-    <col min="178" max="178" width="11.83203125" customWidth="1"/>
-    <col min="179" max="179" width="11" customWidth="1"/>
-    <col min="181" max="181" width="6" style="3" customWidth="1"/>
-    <col min="182" max="183" width="14.83203125" customWidth="1"/>
-    <col min="184" max="184" width="7.1640625" style="3" customWidth="1"/>
-    <col min="185" max="186" width="7.83203125" customWidth="1"/>
-    <col min="187" max="187" width="12.1640625" style="3" customWidth="1"/>
-    <col min="188" max="188" width="12.1640625" customWidth="1"/>
-    <col min="189" max="189" width="12" customWidth="1"/>
-    <col min="190" max="190" width="11.5" customWidth="1"/>
-    <col min="191" max="191" width="14" customWidth="1"/>
-    <col min="192" max="192" width="12.83203125" customWidth="1"/>
-    <col min="193" max="193" width="9.5" customWidth="1"/>
-    <col min="194" max="194" width="13" customWidth="1"/>
-    <col min="195" max="195" width="4.1640625" style="14" customWidth="1"/>
-    <col min="197" max="197" width="7.1640625" customWidth="1"/>
-    <col min="198" max="198" width="10.5" customWidth="1"/>
-    <col min="199" max="199" width="12.5" customWidth="1"/>
-    <col min="201" max="201" width="11.5" customWidth="1"/>
-    <col min="202" max="202" width="9.5" customWidth="1"/>
-    <col min="203" max="203" width="7.1640625" customWidth="1"/>
-    <col min="204" max="205" width="13.6640625" customWidth="1"/>
-    <col min="207" max="207" width="9.1640625" customWidth="1"/>
-    <col min="208" max="208" width="13.1640625" customWidth="1"/>
-    <col min="209" max="209" width="12" customWidth="1"/>
-    <col min="210" max="210" width="12.1640625" customWidth="1"/>
-    <col min="211" max="211" width="5.1640625" style="21" customWidth="1"/>
-    <col min="213" max="213" width="7.5" customWidth="1"/>
-    <col min="214" max="214" width="11" customWidth="1"/>
-    <col min="215" max="215" width="13.5" customWidth="1"/>
-    <col min="216" max="216" width="11.6640625" customWidth="1"/>
-    <col min="217" max="219" width="13.5" customWidth="1"/>
-    <col min="221" max="222" width="13.1640625" customWidth="1"/>
-    <col min="223" max="223" width="11.5" customWidth="1"/>
-    <col min="227" max="227" width="13.83203125" customWidth="1"/>
-    <col min="229" max="229" width="11.5" customWidth="1"/>
-    <col min="230" max="230" width="11.1640625" customWidth="1"/>
-    <col min="231" max="232" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="5" max="5" width="5.5" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" customWidth="1"/>
+    <col min="10" max="11" width="11.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="6" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="8" style="3" customWidth="1"/>
+    <col min="17" max="18" width="7.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.83203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" customWidth="1"/>
+    <col min="21" max="21" width="12.33203125" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="24" max="24" width="11.1640625" customWidth="1"/>
+    <col min="25" max="25" width="9.5" customWidth="1"/>
+    <col min="26" max="26" width="13.83203125" customWidth="1"/>
+    <col min="27" max="27" width="8.83203125" style="5"/>
+    <col min="29" max="29" width="6.83203125" customWidth="1"/>
+    <col min="30" max="30" width="10.83203125" customWidth="1"/>
+    <col min="31" max="31" width="13.83203125" customWidth="1"/>
+    <col min="33" max="35" width="11.5" customWidth="1"/>
+    <col min="38" max="39" width="13.6640625" customWidth="1"/>
+    <col min="42" max="42" width="12.1640625" customWidth="1"/>
+    <col min="43" max="43" width="11.1640625" customWidth="1"/>
+    <col min="44" max="44" width="12.1640625" customWidth="1"/>
+    <col min="46" max="46" width="5.6640625" style="19" customWidth="1"/>
+    <col min="48" max="48" width="6.5" customWidth="1"/>
+    <col min="49" max="49" width="10.83203125" customWidth="1"/>
+    <col min="50" max="50" width="13.83203125" customWidth="1"/>
+    <col min="51" max="51" width="11.83203125" customWidth="1"/>
+    <col min="52" max="54" width="11.5" customWidth="1"/>
+    <col min="55" max="55" width="13.5" customWidth="1"/>
+    <col min="56" max="56" width="11.1640625" customWidth="1"/>
+    <col min="57" max="57" width="10" customWidth="1"/>
+    <col min="58" max="58" width="9.33203125" customWidth="1"/>
+    <col min="61" max="61" width="12.5" customWidth="1"/>
+    <col min="62" max="62" width="10.83203125" customWidth="1"/>
+    <col min="63" max="63" width="12.83203125" customWidth="1"/>
+    <col min="64" max="64" width="4.33203125" style="19" customWidth="1"/>
+    <col min="66" max="66" width="6.1640625" customWidth="1"/>
+    <col min="67" max="67" width="10.83203125" customWidth="1"/>
+    <col min="68" max="68" width="12" customWidth="1"/>
+    <col min="69" max="69" width="8.83203125" customWidth="1"/>
+    <col min="70" max="72" width="11.5" customWidth="1"/>
+    <col min="73" max="73" width="12.33203125" customWidth="1"/>
+    <col min="74" max="74" width="9.1640625" customWidth="1"/>
+    <col min="75" max="75" width="7.33203125" customWidth="1"/>
+    <col min="76" max="76" width="7.83203125" customWidth="1"/>
+    <col min="77" max="77" width="7.5" customWidth="1"/>
+    <col min="78" max="78" width="12.5" customWidth="1"/>
+    <col min="79" max="79" width="10.83203125" customWidth="1"/>
+    <col min="80" max="80" width="11.5" customWidth="1"/>
+    <col min="81" max="81" width="4.5" style="19" customWidth="1"/>
+    <col min="83" max="83" width="5.1640625" customWidth="1"/>
+    <col min="84" max="84" width="13.33203125" customWidth="1"/>
+    <col min="85" max="85" width="12.83203125" customWidth="1"/>
+    <col min="86" max="86" width="10.5" customWidth="1"/>
+    <col min="87" max="89" width="11.33203125" customWidth="1"/>
+    <col min="90" max="90" width="9" customWidth="1"/>
+    <col min="91" max="92" width="13.33203125" customWidth="1"/>
+    <col min="93" max="93" width="9.1640625" customWidth="1"/>
+    <col min="94" max="94" width="7" customWidth="1"/>
+    <col min="97" max="97" width="12.83203125" customWidth="1"/>
+    <col min="98" max="98" width="6.6640625" style="3" customWidth="1"/>
+    <col min="99" max="99" width="12.83203125" customWidth="1"/>
+    <col min="100" max="100" width="10.1640625" customWidth="1"/>
+    <col min="101" max="101" width="11.1640625" customWidth="1"/>
+    <col min="102" max="102" width="12.1640625" customWidth="1"/>
+    <col min="103" max="103" width="3.33203125" customWidth="1"/>
+    <col min="105" max="105" width="7.5" customWidth="1"/>
+    <col min="106" max="106" width="9.6640625" customWidth="1"/>
+    <col min="107" max="107" width="12.1640625" customWidth="1"/>
+    <col min="108" max="108" width="12.33203125" customWidth="1"/>
+    <col min="109" max="111" width="12.1640625" customWidth="1"/>
+    <col min="112" max="112" width="9.1640625" customWidth="1"/>
+    <col min="113" max="114" width="13.33203125" customWidth="1"/>
+    <col min="115" max="115" width="9.1640625" customWidth="1"/>
+    <col min="116" max="116" width="6" customWidth="1"/>
+    <col min="117" max="117" width="7.6640625" customWidth="1"/>
+    <col min="118" max="118" width="7.5" customWidth="1"/>
+    <col min="119" max="119" width="12.83203125" customWidth="1"/>
+    <col min="120" max="120" width="6.6640625" style="3" customWidth="1"/>
+    <col min="121" max="121" width="11.5" customWidth="1"/>
+    <col min="122" max="122" width="10.33203125" customWidth="1"/>
+    <col min="123" max="123" width="13.1640625" customWidth="1"/>
+    <col min="124" max="124" width="12.1640625" customWidth="1"/>
+    <col min="125" max="125" width="4.6640625" style="14" customWidth="1"/>
+    <col min="129" max="129" width="7.5" customWidth="1"/>
+    <col min="130" max="130" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="12.1640625" customWidth="1"/>
+    <col min="133" max="133" width="12.33203125" customWidth="1"/>
+    <col min="134" max="134" width="13.33203125" customWidth="1"/>
+    <col min="135" max="135" width="12.5" customWidth="1"/>
+    <col min="136" max="136" width="10.33203125" customWidth="1"/>
+    <col min="137" max="137" width="6" style="3" customWidth="1"/>
+    <col min="138" max="139" width="13.33203125" customWidth="1"/>
+    <col min="140" max="140" width="7.1640625" style="3" customWidth="1"/>
+    <col min="141" max="142" width="7.83203125" customWidth="1"/>
+    <col min="143" max="143" width="12.1640625" style="3" customWidth="1"/>
+    <col min="144" max="144" width="10.6640625" customWidth="1"/>
+    <col min="145" max="145" width="12.1640625" customWidth="1"/>
+    <col min="146" max="146" width="11" customWidth="1"/>
+    <col min="147" max="147" width="13.1640625" customWidth="1"/>
+    <col min="148" max="148" width="10.83203125" customWidth="1"/>
+    <col min="149" max="149" width="9.83203125" customWidth="1"/>
+    <col min="150" max="150" width="13.1640625" customWidth="1"/>
+    <col min="151" max="151" width="3.83203125" style="14" customWidth="1"/>
+    <col min="155" max="155" width="12.5" customWidth="1"/>
+    <col min="157" max="159" width="11.33203125" customWidth="1"/>
+    <col min="160" max="160" width="9.1640625" customWidth="1"/>
+    <col min="161" max="161" width="6.5" customWidth="1"/>
+    <col min="162" max="163" width="12.83203125" customWidth="1"/>
+    <col min="165" max="165" width="9.1640625" customWidth="1"/>
+    <col min="166" max="166" width="12.1640625" customWidth="1"/>
+    <col min="167" max="167" width="12.83203125" customWidth="1"/>
+    <col min="168" max="168" width="14.1640625" customWidth="1"/>
+    <col min="170" max="170" width="3.6640625" style="15" customWidth="1"/>
+    <col min="172" max="172" width="10" customWidth="1"/>
+    <col min="174" max="174" width="7.5" customWidth="1"/>
+    <col min="175" max="175" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="11.33203125" customWidth="1"/>
+    <col min="178" max="178" width="11.1640625" customWidth="1"/>
+    <col min="179" max="179" width="11.83203125" customWidth="1"/>
+    <col min="180" max="180" width="11" customWidth="1"/>
+    <col min="182" max="182" width="6" style="3" customWidth="1"/>
+    <col min="183" max="184" width="14.83203125" customWidth="1"/>
+    <col min="185" max="185" width="7.1640625" style="3" customWidth="1"/>
+    <col min="186" max="187" width="7.83203125" customWidth="1"/>
+    <col min="188" max="188" width="12.1640625" style="3" customWidth="1"/>
+    <col min="189" max="189" width="12.1640625" customWidth="1"/>
+    <col min="190" max="190" width="12" customWidth="1"/>
+    <col min="191" max="191" width="11.5" customWidth="1"/>
+    <col min="192" max="192" width="14" customWidth="1"/>
+    <col min="193" max="193" width="12.83203125" customWidth="1"/>
+    <col min="194" max="194" width="9.5" customWidth="1"/>
+    <col min="195" max="195" width="13" customWidth="1"/>
+    <col min="196" max="196" width="4.1640625" style="14" customWidth="1"/>
+    <col min="198" max="198" width="7.1640625" customWidth="1"/>
+    <col min="199" max="199" width="10.5" customWidth="1"/>
+    <col min="200" max="200" width="12.5" customWidth="1"/>
+    <col min="202" max="202" width="11.5" customWidth="1"/>
+    <col min="203" max="203" width="9.5" customWidth="1"/>
+    <col min="204" max="204" width="7.1640625" customWidth="1"/>
+    <col min="205" max="206" width="13.6640625" customWidth="1"/>
+    <col min="208" max="208" width="9.1640625" customWidth="1"/>
+    <col min="209" max="209" width="13.1640625" customWidth="1"/>
+    <col min="210" max="210" width="12" customWidth="1"/>
+    <col min="211" max="211" width="12.1640625" customWidth="1"/>
+    <col min="212" max="212" width="5.1640625" style="21" customWidth="1"/>
+    <col min="214" max="214" width="7.5" customWidth="1"/>
+    <col min="215" max="215" width="11" customWidth="1"/>
+    <col min="216" max="216" width="13.5" customWidth="1"/>
+    <col min="217" max="217" width="11.6640625" customWidth="1"/>
+    <col min="218" max="220" width="13.5" customWidth="1"/>
+    <col min="222" max="223" width="13.1640625" customWidth="1"/>
+    <col min="224" max="224" width="11.5" customWidth="1"/>
+    <col min="228" max="228" width="13.83203125" customWidth="1"/>
+    <col min="230" max="230" width="11.5" customWidth="1"/>
+    <col min="231" max="231" width="11.1640625" customWidth="1"/>
+    <col min="232" max="233" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:232" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:233" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>48</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>82</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
       <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>89</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>9</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>88</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>12</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>82</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>0</v>
       </c>
-      <c r="AD1" t="s">
-        <v>1</v>
-      </c>
       <c r="AE1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF1" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>17</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>18</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>2</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>90</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>4</v>
       </c>
-      <c r="AO1" s="3" t="s">
+      <c r="AP1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>29</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>7</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>12</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>82</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>0</v>
       </c>
-      <c r="AW1" t="s">
-        <v>1</v>
-      </c>
       <c r="AX1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY1" t="s">
         <v>23</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>17</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>18</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>19</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>2</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>91</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>20</v>
       </c>
-      <c r="BE1" s="3" t="s">
+      <c r="BF1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="BF1" s="3" t="s">
+      <c r="BG1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>4</v>
       </c>
-      <c r="BH1" s="3" t="s">
+      <c r="BI1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>81</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>7</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>12</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>85</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>0</v>
       </c>
-      <c r="BO1" t="s">
-        <v>1</v>
-      </c>
       <c r="BP1" t="s">
+        <v>1</v>
+      </c>
+      <c r="BQ1" t="s">
         <v>23</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>17</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>18</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>19</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>2</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>20</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>4</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>81</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>7</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>12</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>82</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>0</v>
       </c>
-      <c r="CF1" t="s">
-        <v>1</v>
-      </c>
       <c r="CG1" t="s">
+        <v>1</v>
+      </c>
+      <c r="CH1" t="s">
         <v>23</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>17</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>18</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>19</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>41</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>2</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>90</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>20</v>
       </c>
-      <c r="CO1" s="3" t="s">
+      <c r="CP1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="CP1" s="3" t="s">
+      <c r="CQ1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>4</v>
       </c>
-      <c r="CR1" s="3" t="s">
+      <c r="CS1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="CS1" s="3" t="s">
+      <c r="CT1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="CT1" s="3" t="s">
+      <c r="CU1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>81</v>
       </c>
-      <c r="CV1" s="3" t="s">
+      <c r="CW1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>7</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>12</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>82</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>0</v>
       </c>
-      <c r="DB1" t="s">
-        <v>1</v>
-      </c>
       <c r="DC1" t="s">
+        <v>1</v>
+      </c>
+      <c r="DD1" t="s">
         <v>23</v>
       </c>
-      <c r="DD1" t="s">
+      <c r="DE1" t="s">
         <v>17</v>
       </c>
-      <c r="DE1" t="s">
+      <c r="DF1" t="s">
         <v>18</v>
       </c>
-      <c r="DF1" t="s">
+      <c r="DG1" t="s">
         <v>19</v>
       </c>
-      <c r="DG1" t="s">
+      <c r="DH1" t="s">
         <v>41</v>
       </c>
-      <c r="DH1" t="s">
+      <c r="DI1" t="s">
         <v>2</v>
       </c>
-      <c r="DI1" t="s">
+      <c r="DJ1" t="s">
         <v>90</v>
       </c>
-      <c r="DJ1" t="s">
+      <c r="DK1" t="s">
         <v>20</v>
       </c>
-      <c r="DK1" s="3" t="s">
+      <c r="DL1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="DL1" s="3" t="s">
+      <c r="DM1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="DM1" t="s">
+      <c r="DN1" t="s">
         <v>4</v>
       </c>
-      <c r="DN1" s="3" t="s">
+      <c r="DO1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="DO1" s="3" t="s">
+      <c r="DP1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="DP1" s="3" t="s">
+      <c r="DQ1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="DQ1" t="s">
+      <c r="DR1" t="s">
         <v>81</v>
       </c>
-      <c r="DR1" s="3" t="s">
+      <c r="DS1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="DS1" t="s">
+      <c r="DT1" t="s">
         <v>7</v>
       </c>
-      <c r="DU1" t="s">
+      <c r="DV1" t="s">
         <v>12</v>
       </c>
-      <c r="DV1" t="s">
+      <c r="DW1" t="s">
         <v>48</v>
       </c>
-      <c r="DW1" t="s">
+      <c r="DX1" t="s">
         <v>49</v>
       </c>
-      <c r="DX1" t="s">
+      <c r="DY1" t="s">
         <v>82</v>
       </c>
-      <c r="DY1" t="s">
+      <c r="DZ1" t="s">
         <v>0</v>
       </c>
-      <c r="DZ1" t="s">
-        <v>1</v>
-      </c>
       <c r="EA1" t="s">
+        <v>1</v>
+      </c>
+      <c r="EB1" t="s">
         <v>23</v>
       </c>
-      <c r="EB1" t="s">
+      <c r="EC1" t="s">
         <v>17</v>
       </c>
-      <c r="EC1" t="s">
+      <c r="ED1" t="s">
         <v>18</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="EE1" t="s">
         <v>19</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EF1" t="s">
         <v>20</v>
       </c>
-      <c r="EF1" s="3" t="s">
+      <c r="EG1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="EG1" t="s">
+      <c r="EH1" t="s">
         <v>2</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EI1" t="s">
         <v>89</v>
       </c>
-      <c r="EI1" s="3" t="s">
+      <c r="EJ1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EK1" t="s">
         <v>4</v>
       </c>
-      <c r="EK1" s="3" t="s">
+      <c r="EL1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="EL1" s="3" t="s">
+      <c r="EM1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EN1" t="s">
         <v>6</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="EO1" t="s">
         <v>7</v>
       </c>
-      <c r="EO1" t="s">
+      <c r="EP1" t="s">
         <v>8</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="EQ1" t="s">
         <v>9</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ER1" t="s">
         <v>29</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="ES1" t="s">
         <v>11</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="ET1" t="s">
         <v>88</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EV1" t="s">
         <v>12</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EW1" t="s">
         <v>82</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EX1" t="s">
         <v>0</v>
       </c>
-      <c r="EX1" t="s">
-        <v>1</v>
-      </c>
       <c r="EY1" t="s">
+        <v>1</v>
+      </c>
+      <c r="EZ1" t="s">
         <v>23</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FA1" t="s">
         <v>17</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FB1" t="s">
         <v>18</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FC1" t="s">
         <v>19</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FD1" t="s">
         <v>20</v>
       </c>
-      <c r="FD1" s="3" t="s">
+      <c r="FE1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="FE1" t="s">
+      <c r="FF1" t="s">
         <v>2</v>
       </c>
-      <c r="FF1" t="s">
+      <c r="FG1" t="s">
         <v>90</v>
       </c>
-      <c r="FG1" s="3" t="s">
+      <c r="FH1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="FH1" t="s">
+      <c r="FI1" t="s">
         <v>4</v>
       </c>
-      <c r="FI1" s="3" t="s">
+      <c r="FJ1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="FJ1" t="s">
+      <c r="FK1" t="s">
         <v>29</v>
       </c>
-      <c r="FK1" t="s">
+      <c r="FL1" t="s">
         <v>7</v>
       </c>
-      <c r="FN1" t="s">
+      <c r="FO1" t="s">
         <v>12</v>
       </c>
-      <c r="FO1" t="s">
+      <c r="FP1" t="s">
         <v>48</v>
       </c>
-      <c r="FP1" t="s">
+      <c r="FQ1" t="s">
         <v>49</v>
       </c>
-      <c r="FQ1" t="s">
+      <c r="FR1" t="s">
         <v>82</v>
       </c>
-      <c r="FR1" t="s">
+      <c r="FS1" t="s">
         <v>0</v>
       </c>
-      <c r="FS1" t="s">
-        <v>1</v>
-      </c>
       <c r="FT1" t="s">
+        <v>1</v>
+      </c>
+      <c r="FU1" t="s">
         <v>23</v>
       </c>
-      <c r="FU1" t="s">
+      <c r="FV1" t="s">
         <v>17</v>
       </c>
-      <c r="FV1" t="s">
+      <c r="FW1" t="s">
         <v>18</v>
       </c>
-      <c r="FW1" t="s">
+      <c r="FX1" t="s">
         <v>19</v>
       </c>
-      <c r="FX1" t="s">
+      <c r="FY1" t="s">
         <v>20</v>
       </c>
-      <c r="FY1" s="3" t="s">
+      <c r="FZ1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="FZ1" t="s">
+      <c r="GA1" t="s">
         <v>2</v>
       </c>
-      <c r="GA1" t="s">
+      <c r="GB1" t="s">
         <v>89</v>
       </c>
-      <c r="GB1" s="3" t="s">
+      <c r="GC1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="GC1" t="s">
+      <c r="GD1" t="s">
         <v>4</v>
       </c>
-      <c r="GD1" s="3" t="s">
+      <c r="GE1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="GE1" s="3" t="s">
+      <c r="GF1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="GF1" t="s">
+      <c r="GG1" t="s">
         <v>6</v>
       </c>
-      <c r="GG1" t="s">
+      <c r="GH1" t="s">
         <v>7</v>
       </c>
-      <c r="GH1" t="s">
+      <c r="GI1" t="s">
         <v>8</v>
       </c>
-      <c r="GI1" t="s">
+      <c r="GJ1" t="s">
         <v>9</v>
       </c>
-      <c r="GJ1" t="s">
+      <c r="GK1" t="s">
         <v>29</v>
       </c>
-      <c r="GK1" t="s">
+      <c r="GL1" t="s">
         <v>11</v>
       </c>
-      <c r="GL1" t="s">
+      <c r="GM1" t="s">
         <v>88</v>
       </c>
-      <c r="GN1" t="s">
+      <c r="GO1" t="s">
         <v>12</v>
       </c>
-      <c r="GO1" t="s">
+      <c r="GP1" t="s">
         <v>82</v>
       </c>
-      <c r="GP1" t="s">
+      <c r="GQ1" t="s">
         <v>0</v>
       </c>
-      <c r="GQ1" t="s">
-        <v>1</v>
-      </c>
       <c r="GR1" t="s">
+        <v>1</v>
+      </c>
+      <c r="GS1" t="s">
         <v>23</v>
       </c>
-      <c r="GS1" t="s">
+      <c r="GT1" t="s">
         <v>17</v>
       </c>
-      <c r="GT1" t="s">
+      <c r="GU1" t="s">
         <v>20</v>
       </c>
-      <c r="GU1" s="3" t="s">
+      <c r="GV1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="GV1" t="s">
+      <c r="GW1" t="s">
         <v>2</v>
       </c>
-      <c r="GW1" t="s">
+      <c r="GX1" t="s">
         <v>90</v>
       </c>
-      <c r="GX1" s="3" t="s">
+      <c r="GY1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="GY1" t="s">
+      <c r="GZ1" t="s">
         <v>4</v>
       </c>
-      <c r="GZ1" s="3" t="s">
+      <c r="HA1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="HA1" t="s">
+      <c r="HB1" t="s">
         <v>29</v>
       </c>
-      <c r="HB1" t="s">
+      <c r="HC1" t="s">
         <v>7</v>
       </c>
-      <c r="HD1" t="s">
+      <c r="HE1" t="s">
         <v>12</v>
       </c>
-      <c r="HE1" t="s">
+      <c r="HF1" t="s">
         <v>82</v>
       </c>
-      <c r="HF1" t="s">
+      <c r="HG1" t="s">
         <v>0</v>
       </c>
-      <c r="HG1" t="s">
-        <v>1</v>
-      </c>
       <c r="HH1" t="s">
+        <v>1</v>
+      </c>
+      <c r="HI1" t="s">
         <v>23</v>
       </c>
-      <c r="HI1" t="s">
+      <c r="HJ1" t="s">
         <v>17</v>
       </c>
-      <c r="HJ1" t="s">
+      <c r="HK1" t="s">
         <v>18</v>
       </c>
-      <c r="HK1" t="s">
+      <c r="HL1" t="s">
         <v>19</v>
       </c>
-      <c r="HL1" t="s">
+      <c r="HM1" t="s">
         <v>41</v>
       </c>
-      <c r="HM1" t="s">
+      <c r="HN1" t="s">
         <v>2</v>
       </c>
-      <c r="HN1" t="s">
+      <c r="HO1" t="s">
         <v>90</v>
       </c>
-      <c r="HO1" t="s">
+      <c r="HP1" t="s">
         <v>20</v>
       </c>
-      <c r="HP1" s="3" t="s">
+      <c r="HQ1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="HQ1" s="3" t="s">
+      <c r="HR1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="HR1" t="s">
+      <c r="HS1" t="s">
         <v>4</v>
       </c>
-      <c r="HS1" s="3" t="s">
+      <c r="HT1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="HT1" s="3" t="s">
+      <c r="HU1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="HU1" s="3" t="s">
+      <c r="HV1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="HV1" t="s">
+      <c r="HW1" t="s">
         <v>81</v>
       </c>
-      <c r="HW1" s="3" t="s">
+      <c r="HX1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="HX1" t="s">
+      <c r="HY1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:232" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:233" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>8000</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>801</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <v>220</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1">
+      <c r="Q2" s="1">
         <v>109</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="R2" s="1">
         <v>45</v>
       </c>
-      <c r="R2" s="4">
+      <c r="S2" s="4">
         <v>11</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>23</v>
       </c>
-      <c r="T2" s="18">
+      <c r="U2" s="18">
         <v>8</v>
       </c>
-      <c r="U2" s="1">
+      <c r="V2" s="1">
         <v>16</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>24</v>
       </c>
-      <c r="W2" s="1">
+      <c r="X2" s="1">
         <v>1.2</v>
       </c>
-      <c r="X2" s="1">
+      <c r="Y2" s="1">
         <v>65</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Z2" s="1">
         <v>16</v>
       </c>
-      <c r="Z2" s="6"/>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AI2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AJ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AL2" s="1">
         <v>800.2</v>
       </c>
-      <c r="AL2" s="1">
+      <c r="AM2" s="1">
         <v>450</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AO2" s="1">
         <v>102</v>
       </c>
-      <c r="AO2" s="4">
+      <c r="AP2" s="4">
         <v>8</v>
       </c>
-      <c r="AP2" s="1">
-        <v>1</v>
-      </c>
       <c r="AQ2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="1">
         <v>5</v>
       </c>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="1" t="s">
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AV2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AX2" s="1" t="s">
+      <c r="AY2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BB2" s="1">
+      <c r="BC2" s="1">
         <v>450</v>
       </c>
-      <c r="BC2" s="1">
+      <c r="BD2" s="1">
         <v>600</v>
       </c>
-      <c r="BD2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE2" s="4" t="s">
+      <c r="BE2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="BF2" s="4" t="s">
+      <c r="BG2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BG2" s="1">
+      <c r="BH2" s="1">
         <v>102</v>
       </c>
-      <c r="BH2" s="4">
+      <c r="BI2" s="4">
         <v>8</v>
       </c>
-      <c r="BI2" s="1">
+      <c r="BJ2" s="1">
         <v>0.08</v>
       </c>
-      <c r="BJ2" s="1">
+      <c r="BK2" s="1">
         <v>5</v>
       </c>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="1" t="s">
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="BM2" s="1" t="s">
+      <c r="BN2" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="BN2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BP2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="BT2" s="1">
+      <c r="BU2" s="1">
         <v>450</v>
       </c>
-      <c r="BU2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="BX2" s="1">
+      <c r="BY2" s="1">
         <v>102</v>
       </c>
-      <c r="BY2" s="4">
+      <c r="BZ2" s="4">
         <v>8</v>
       </c>
-      <c r="BZ2" s="1">
+      <c r="CA2" s="1">
         <v>0.08</v>
       </c>
-      <c r="CA2" s="1">
+      <c r="CB2" s="1">
         <v>5</v>
       </c>
-      <c r="CB2" s="20"/>
-      <c r="CC2" s="11" t="s">
+      <c r="CC2" s="20"/>
+      <c r="CD2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="CD2" s="11" t="s">
+      <c r="CE2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="CE2" s="11" t="s">
+      <c r="CF2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="CF2" s="11" t="s">
+      <c r="CG2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="CG2" s="11" t="s">
+      <c r="CH2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="CH2" s="11" t="s">
+      <c r="CI2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="CI2" s="11"/>
       <c r="CJ2" s="11"/>
-      <c r="CK2" s="11">
+      <c r="CK2" s="11"/>
+      <c r="CL2" s="11">
         <v>96</v>
       </c>
-      <c r="CL2" s="11">
+      <c r="CM2" s="11">
         <v>400</v>
       </c>
-      <c r="CM2" s="11">
+      <c r="CN2" s="11">
         <v>92</v>
       </c>
-      <c r="CN2" s="11">
-        <v>1</v>
-      </c>
-      <c r="CO2" s="12" t="s">
+      <c r="CO2" s="11">
+        <v>1</v>
+      </c>
+      <c r="CP2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="CP2" s="12" t="s">
+      <c r="CQ2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="CQ2" s="11">
+      <c r="CR2" s="11">
         <v>102</v>
       </c>
-      <c r="CR2" s="12">
+      <c r="CS2" s="12">
         <v>12</v>
       </c>
-      <c r="CS2" s="12">
+      <c r="CT2" s="12">
         <v>24</v>
       </c>
-      <c r="CT2" s="12">
+      <c r="CU2" s="12">
         <v>0.02</v>
       </c>
-      <c r="CU2" s="11">
+      <c r="CV2" s="11">
         <v>0.08</v>
       </c>
-      <c r="CV2" s="11">
+      <c r="CW2" s="11">
         <v>0</v>
       </c>
-      <c r="CW2" s="11">
+      <c r="CX2" s="11">
         <v>5</v>
       </c>
-      <c r="CX2" s="2"/>
-      <c r="CY2" s="11" t="s">
+      <c r="CY2" s="2"/>
+      <c r="CZ2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="CZ2" s="11" t="s">
+      <c r="DA2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="DA2" s="11" t="s">
+      <c r="DB2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="DB2" s="11" t="s">
+      <c r="DC2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="DC2" s="11" t="s">
+      <c r="DD2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="DD2" s="11" t="s">
+      <c r="DE2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="DE2" s="11"/>
       <c r="DF2" s="11"/>
-      <c r="DG2" s="11">
+      <c r="DG2" s="11"/>
+      <c r="DH2" s="11">
         <v>120</v>
       </c>
-      <c r="DH2" s="11">
+      <c r="DI2" s="11">
         <v>400</v>
       </c>
-      <c r="DI2" s="11">
+      <c r="DJ2" s="11">
         <v>62</v>
       </c>
-      <c r="DJ2" s="11">
-        <v>1</v>
-      </c>
-      <c r="DK2" s="12" t="s">
+      <c r="DK2" s="11">
+        <v>1</v>
+      </c>
+      <c r="DL2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="DL2" s="12" t="s">
+      <c r="DM2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="DM2" s="11">
+      <c r="DN2" s="11">
         <v>102</v>
       </c>
-      <c r="DN2" s="12">
+      <c r="DO2" s="12">
         <v>12</v>
       </c>
-      <c r="DO2" s="12">
+      <c r="DP2" s="12">
         <v>37</v>
       </c>
-      <c r="DP2" s="12">
+      <c r="DQ2" s="12">
         <v>0.02</v>
       </c>
-      <c r="DQ2" s="11">
+      <c r="DR2" s="11">
         <v>0.08</v>
       </c>
-      <c r="DR2" s="11">
+      <c r="DS2" s="11">
         <v>0</v>
       </c>
-      <c r="DS2" s="11">
+      <c r="DT2" s="11">
         <v>5</v>
       </c>
-      <c r="DT2" s="9"/>
-      <c r="DU2" s="1" t="s">
+      <c r="DU2" s="9"/>
+      <c r="DV2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="DV2" s="1" t="s">
+      <c r="DW2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="DW2" s="1">
+      <c r="DX2" s="1">
         <v>10000</v>
       </c>
-      <c r="DX2" s="1" t="s">
+      <c r="DY2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="DY2" s="1" t="s">
+      <c r="DZ2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="DZ2" s="1" t="s">
+      <c r="EA2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="EA2" s="1" t="s">
+      <c r="EB2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="EB2" s="1" t="s">
+      <c r="EC2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="EC2" s="1" t="s">
+      <c r="ED2" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="EE2" s="1">
+      <c r="EF2" s="1">
         <v>2</v>
       </c>
-      <c r="EF2" s="4" t="s">
+      <c r="EG2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="EG2" s="1">
+      <c r="EH2" s="1">
         <v>800.2</v>
       </c>
-      <c r="EH2" s="1">
+      <c r="EI2" s="1">
         <v>150</v>
       </c>
-      <c r="EI2" s="4" t="s">
+      <c r="EJ2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="EJ2" s="1">
+      <c r="EK2" s="1">
         <v>109</v>
       </c>
-      <c r="EK2" s="1">
+      <c r="EL2" s="1">
         <v>45</v>
       </c>
-      <c r="EL2" s="4">
+      <c r="EM2" s="4">
         <v>11</v>
       </c>
-      <c r="EM2" s="1">
+      <c r="EN2" s="1">
         <v>23</v>
       </c>
-      <c r="EN2" s="1">
+      <c r="EO2" s="1">
         <v>8</v>
       </c>
-      <c r="EO2" s="1">
+      <c r="EP2" s="1">
         <v>16</v>
       </c>
-      <c r="EP2" s="1">
+      <c r="EQ2" s="1">
         <v>24</v>
       </c>
-      <c r="EQ2" s="1">
+      <c r="ER2" s="1">
         <v>1.2</v>
       </c>
-      <c r="ER2" s="1">
+      <c r="ES2" s="1">
         <v>65</v>
       </c>
-      <c r="ES2" s="1">
+      <c r="ET2" s="1">
         <v>16</v>
       </c>
-      <c r="ET2" s="9"/>
-      <c r="EU2" s="1" t="s">
+      <c r="EU2" s="9"/>
+      <c r="EV2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="EV2" s="1" t="s">
+      <c r="EW2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="EW2" s="1" t="s">
+      <c r="EX2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="EX2" s="1" t="s">
+      <c r="EY2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="EY2" s="1" t="s">
+      <c r="EZ2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="EZ2" s="1" t="s">
+      <c r="FA2" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="FC2" s="1">
-        <v>1</v>
-      </c>
-      <c r="FD2" s="4" t="s">
+      <c r="FD2" s="1">
+        <v>1</v>
+      </c>
+      <c r="FE2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="FE2" s="1">
+      <c r="FF2" s="1">
         <v>1000</v>
       </c>
-      <c r="FF2" s="1">
+      <c r="FG2" s="1">
         <v>550</v>
       </c>
-      <c r="FG2" s="17" t="s">
+      <c r="FH2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="FH2" s="1">
+      <c r="FI2" s="1">
         <v>102</v>
       </c>
-      <c r="FI2" s="4">
+      <c r="FJ2" s="4">
         <v>11</v>
       </c>
-      <c r="FJ2" s="1">
-        <v>1</v>
-      </c>
       <c r="FK2" s="1">
+        <v>1</v>
+      </c>
+      <c r="FL2" s="1">
         <v>5</v>
       </c>
-      <c r="FM2" s="16"/>
-      <c r="FN2" s="1" t="s">
+      <c r="FN2" s="16"/>
+      <c r="FO2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="FO2" s="1" t="s">
+      <c r="FP2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="FP2" s="1">
+      <c r="FQ2" s="1">
         <v>1200</v>
       </c>
-      <c r="FQ2" s="1" t="s">
+      <c r="FR2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="FR2" s="1" t="s">
+      <c r="FS2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="FS2" s="1" t="s">
+      <c r="FT2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="FT2" s="1" t="s">
+      <c r="FU2" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="FU2" s="1" t="s">
+      <c r="FV2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="FV2" s="1" t="s">
+      <c r="FW2" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="FX2" s="1">
-        <v>1</v>
-      </c>
-      <c r="FY2" s="4" t="s">
+      <c r="FY2" s="1">
+        <v>1</v>
+      </c>
+      <c r="FZ2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="FZ2" s="1">
+      <c r="GA2" s="1">
         <v>800.2</v>
       </c>
-      <c r="GA2" s="1">
+      <c r="GB2" s="1">
         <v>160</v>
       </c>
-      <c r="GB2" s="17" t="s">
+      <c r="GC2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="GC2" s="1">
+      <c r="GD2" s="1">
         <v>109</v>
       </c>
-      <c r="GD2" s="1">
+      <c r="GE2" s="1">
         <v>45</v>
       </c>
-      <c r="GE2" s="4">
+      <c r="GF2" s="4">
         <v>11</v>
       </c>
-      <c r="GF2" s="1">
+      <c r="GG2" s="1">
         <v>23</v>
       </c>
-      <c r="GG2" s="1">
+      <c r="GH2" s="1">
         <v>8</v>
       </c>
-      <c r="GH2" s="1">
+      <c r="GI2" s="1">
         <v>16</v>
       </c>
-      <c r="GI2" s="1">
+      <c r="GJ2" s="1">
         <v>24</v>
       </c>
-      <c r="GJ2" s="1">
+      <c r="GK2" s="1">
         <v>1.2</v>
       </c>
-      <c r="GK2" s="1">
+      <c r="GL2" s="1">
         <v>65</v>
       </c>
-      <c r="GL2" s="1">
+      <c r="GM2" s="1">
         <v>16</v>
       </c>
-      <c r="GM2" s="9"/>
-      <c r="GN2" s="1" t="s">
+      <c r="GN2" s="9"/>
+      <c r="GO2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="GO2" s="1" t="s">
+      <c r="GP2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="GP2" s="1" t="s">
+      <c r="GQ2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="GQ2" s="1" t="s">
+      <c r="GR2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="GR2" s="1" t="s">
+      <c r="GS2" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="GS2" s="1" t="s">
+      <c r="GT2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="GT2" s="1">
-        <v>1</v>
-      </c>
-      <c r="GU2" s="4" t="s">
+      <c r="GU2" s="1">
+        <v>1</v>
+      </c>
+      <c r="GV2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="GV2" s="1">
+      <c r="GW2" s="1">
         <v>1000</v>
       </c>
-      <c r="GW2" s="1">
+      <c r="GX2" s="1">
         <v>500</v>
       </c>
-      <c r="GX2" s="17" t="s">
+      <c r="GY2" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="GY2" s="1">
+      <c r="GZ2" s="1">
         <v>102</v>
       </c>
-      <c r="GZ2" s="4">
+      <c r="HA2" s="4">
         <v>11</v>
       </c>
-      <c r="HA2" s="1">
-        <v>1</v>
-      </c>
       <c r="HB2" s="1">
+        <v>1</v>
+      </c>
+      <c r="HC2" s="1">
         <v>5</v>
       </c>
-      <c r="HC2" s="22"/>
-      <c r="HD2" s="11" t="s">
+      <c r="HD2" s="22"/>
+      <c r="HE2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="HE2" s="11" t="s">
+      <c r="HF2" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="HF2" s="11" t="s">
+      <c r="HG2" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="HG2" s="11" t="s">
+      <c r="HH2" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="HH2" s="11" t="s">
+      <c r="HI2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="HI2" s="11" t="s">
+      <c r="HJ2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="HJ2" s="11"/>
       <c r="HK2" s="11"/>
-      <c r="HL2" s="11">
+      <c r="HL2" s="11"/>
+      <c r="HM2" s="11">
         <v>80</v>
       </c>
-      <c r="HM2" s="11">
+      <c r="HN2" s="11">
         <v>1000</v>
       </c>
-      <c r="HN2" s="11">
+      <c r="HO2" s="11">
         <v>90</v>
       </c>
-      <c r="HO2" s="11">
-        <v>1</v>
-      </c>
-      <c r="HP2" s="12" t="s">
+      <c r="HP2" s="11">
+        <v>1</v>
+      </c>
+      <c r="HQ2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="HQ2" s="12" t="s">
+      <c r="HR2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="HR2" s="11">
+      <c r="HS2" s="11">
         <v>102</v>
       </c>
-      <c r="HS2" s="12">
+      <c r="HT2" s="12">
         <v>12</v>
       </c>
-      <c r="HT2" s="12">
+      <c r="HU2" s="12">
         <v>37</v>
       </c>
-      <c r="HU2" s="12">
+      <c r="HV2" s="12">
         <v>0.02</v>
       </c>
-      <c r="HV2" s="11">
+      <c r="HW2" s="11">
         <v>0.08</v>
       </c>
-      <c r="HW2" s="11">
+      <c r="HX2" s="11">
         <v>0</v>
       </c>
-      <c r="HX2" s="11">
+      <c r="HY2" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:232" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:233" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>2</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>100</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>0</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>15</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="R3" s="1">
         <v>0</v>
       </c>
-      <c r="R3" s="4">
+      <c r="S3" s="4">
         <v>5</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>34</v>
       </c>
-      <c r="T3" s="18">
+      <c r="U3" s="18">
         <v>9</v>
       </c>
-      <c r="U3" s="1">
+      <c r="V3" s="1">
         <v>9</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>12</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>2</v>
       </c>
-      <c r="X3" s="1">
+      <c r="Y3" s="1">
         <v>25</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Z3" s="1">
         <v>0</v>
       </c>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AI3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="4" t="s">
+      <c r="AJ3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AK3" s="1">
+      <c r="AL3" s="1">
         <v>300</v>
       </c>
-      <c r="AL3" s="1">
+      <c r="AM3" s="1">
         <v>0</v>
       </c>
-      <c r="AM3" s="4" t="s">
+      <c r="AN3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AN3" s="1">
+      <c r="AO3" s="1">
         <v>89</v>
       </c>
-      <c r="AO3" s="4">
+      <c r="AP3" s="4">
         <v>8</v>
       </c>
-      <c r="AP3" s="1">
+      <c r="AQ3" s="1">
         <v>3</v>
       </c>
-      <c r="AQ3" s="1">
+      <c r="AR3" s="1">
         <v>9</v>
       </c>
-      <c r="AS3" s="20"/>
-      <c r="AT3" s="1" t="s">
+      <c r="AT3" s="20"/>
+      <c r="AU3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AV3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AV3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AY3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BB3" s="1">
+      <c r="BC3" s="1">
         <v>780</v>
       </c>
-      <c r="BC3" s="1">
+      <c r="BD3" s="1">
         <v>500</v>
       </c>
-      <c r="BD3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BE3" s="4" t="s">
+      <c r="BE3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BF3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="BF3" s="4" t="s">
+      <c r="BG3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="BG3" s="1">
+      <c r="BH3" s="1">
         <v>89</v>
       </c>
-      <c r="BH3" s="4">
+      <c r="BI3" s="4">
         <v>8</v>
       </c>
-      <c r="BI3" s="1">
+      <c r="BJ3" s="1">
         <v>0.09</v>
       </c>
-      <c r="BJ3" s="1">
+      <c r="BK3" s="1">
         <v>4</v>
       </c>
-      <c r="BK3" s="20"/>
-      <c r="BL3" s="1" t="s">
+      <c r="BL3" s="20"/>
+      <c r="BM3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="BM3" s="1" t="s">
+      <c r="BN3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="BN3" s="1" t="s">
+      <c r="BO3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="BO3" s="1" t="s">
+      <c r="BP3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BP3" s="1" t="s">
+      <c r="BQ3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BQ3" s="1" t="s">
+      <c r="BR3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="BT3" s="1">
+      <c r="BU3" s="1">
         <v>500</v>
       </c>
-      <c r="BU3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BV3" s="4" t="s">
+      <c r="BV3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BW3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="BW3" s="4" t="s">
+      <c r="BX3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="BX3" s="1">
+      <c r="BY3" s="1">
         <v>89</v>
       </c>
-      <c r="BY3" s="4">
+      <c r="BZ3" s="4">
         <v>8</v>
       </c>
-      <c r="BZ3" s="1">
+      <c r="CA3" s="1">
         <v>0.09</v>
       </c>
-      <c r="CA3" s="1">
+      <c r="CB3" s="1">
         <v>4</v>
       </c>
-      <c r="CB3" s="20"/>
-      <c r="CC3" s="11" t="s">
+      <c r="CC3" s="20"/>
+      <c r="CD3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="CD3" s="11" t="s">
+      <c r="CE3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="CE3" s="11" t="s">
+      <c r="CF3" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="CF3" s="11" t="s">
+      <c r="CG3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="CG3" s="11" t="s">
+      <c r="CH3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="CH3" s="11" t="s">
+      <c r="CI3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="CI3" s="11"/>
       <c r="CJ3" s="11"/>
-      <c r="CK3" s="11">
+      <c r="CK3" s="11"/>
+      <c r="CL3" s="11">
         <v>96</v>
       </c>
-      <c r="CL3" s="11">
+      <c r="CM3" s="11">
         <v>300</v>
       </c>
-      <c r="CM3" s="11">
+      <c r="CN3" s="11">
         <v>92</v>
       </c>
-      <c r="CN3" s="11">
-        <v>1</v>
-      </c>
-      <c r="CO3" s="12" t="s">
+      <c r="CO3" s="11">
+        <v>1</v>
+      </c>
+      <c r="CP3" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="CP3" s="12" t="s">
+      <c r="CQ3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="CQ3" s="11">
+      <c r="CR3" s="11">
         <v>89</v>
       </c>
-      <c r="CR3" s="12">
+      <c r="CS3" s="12">
         <v>12</v>
       </c>
-      <c r="CS3" s="12">
+      <c r="CT3" s="12">
         <v>0</v>
       </c>
-      <c r="CT3" s="12">
+      <c r="CU3" s="12">
         <v>0.02</v>
       </c>
-      <c r="CU3" s="11">
+      <c r="CV3" s="11">
         <v>0.09</v>
       </c>
-      <c r="CV3" s="11">
-        <v>1</v>
-      </c>
-      <c r="CW3" s="11"/>
-      <c r="CX3" s="2"/>
-      <c r="CY3" s="11" t="s">
+      <c r="CW3" s="11">
+        <v>1</v>
+      </c>
+      <c r="CX3" s="11"/>
+      <c r="CY3" s="2"/>
+      <c r="CZ3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="CZ3" s="11" t="s">
+      <c r="DA3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="DA3" s="11" t="s">
+      <c r="DB3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="DB3" s="11" t="s">
+      <c r="DC3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="DC3" s="11" t="s">
+      <c r="DD3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="DD3" s="11" t="s">
+      <c r="DE3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="DE3" s="11"/>
       <c r="DF3" s="11"/>
-      <c r="DG3" s="11">
+      <c r="DG3" s="11"/>
+      <c r="DH3" s="11">
         <v>120</v>
       </c>
-      <c r="DH3" s="11">
+      <c r="DI3" s="11">
         <v>300</v>
       </c>
-      <c r="DI3" s="11">
+      <c r="DJ3" s="11">
         <v>65</v>
       </c>
-      <c r="DJ3" s="11">
-        <v>1</v>
-      </c>
-      <c r="DK3" s="12" t="s">
+      <c r="DK3" s="11">
+        <v>1</v>
+      </c>
+      <c r="DL3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="DL3" s="12" t="s">
+      <c r="DM3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="DM3" s="11">
+      <c r="DN3" s="11">
         <v>89</v>
       </c>
-      <c r="DN3" s="12">
+      <c r="DO3" s="12">
         <v>12</v>
       </c>
-      <c r="DO3" s="12">
+      <c r="DP3" s="12">
         <v>0</v>
       </c>
-      <c r="DP3" s="12">
+      <c r="DQ3" s="12">
         <v>0.02</v>
       </c>
-      <c r="DQ3" s="11">
+      <c r="DR3" s="11">
         <v>0.09</v>
       </c>
-      <c r="DR3" s="11">
-        <v>1</v>
-      </c>
       <c r="DS3" s="11">
+        <v>1</v>
+      </c>
+      <c r="DT3" s="11">
         <v>0</v>
       </c>
-      <c r="DT3" s="9"/>
-      <c r="DU3" s="1" t="s">
+      <c r="DU3" s="9"/>
+      <c r="DV3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="DX3" s="1" t="s">
+      <c r="DY3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="DY3" s="1" t="s">
+      <c r="DZ3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="DZ3" s="1" t="s">
+      <c r="EA3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="EA3" s="1" t="s">
+      <c r="EB3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="EB3" s="1" t="s">
+      <c r="EC3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="EC3" s="1" t="s">
+      <c r="ED3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="EE3" s="1">
+      <c r="EF3" s="1">
         <v>2</v>
       </c>
-      <c r="EF3" s="4" t="s">
+      <c r="EG3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="EG3" s="1">
+      <c r="EH3" s="1">
         <v>100</v>
       </c>
-      <c r="EH3" s="1">
+      <c r="EI3" s="1">
         <v>0</v>
       </c>
-      <c r="EI3" s="4" t="s">
+      <c r="EJ3" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="EJ3" s="1">
+      <c r="EK3" s="1">
         <v>15</v>
       </c>
-      <c r="EK3" s="1">
+      <c r="EL3" s="1">
         <v>0</v>
       </c>
-      <c r="EL3" s="4">
+      <c r="EM3" s="4">
         <v>5</v>
       </c>
-      <c r="EM3" s="1">
+      <c r="EN3" s="1">
         <v>56</v>
-      </c>
-      <c r="EN3" s="1">
-        <v>9</v>
       </c>
       <c r="EO3" s="1">
         <v>9</v>
       </c>
       <c r="EP3" s="1">
+        <v>9</v>
+      </c>
+      <c r="EQ3" s="1">
         <v>12</v>
       </c>
-      <c r="EQ3" s="1">
+      <c r="ER3" s="1">
         <v>2</v>
       </c>
-      <c r="ER3" s="1">
+      <c r="ES3" s="1">
         <v>25</v>
       </c>
-      <c r="ES3" s="1">
+      <c r="ET3" s="1">
         <v>0</v>
       </c>
-      <c r="ET3" s="9"/>
-      <c r="EU3" s="1" t="s">
+      <c r="EU3" s="9"/>
+      <c r="EV3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="EV3" s="1" t="s">
+      <c r="EW3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="EW3" s="1" t="s">
+      <c r="EX3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="EX3" s="1" t="s">
+      <c r="EY3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="FD3" s="4"/>
-      <c r="FE3" s="1">
+      <c r="FE3" s="4"/>
+      <c r="FF3" s="1">
         <v>0</v>
       </c>
-      <c r="FG3" s="17"/>
-      <c r="FI3" s="4"/>
-      <c r="FM3" s="16"/>
-      <c r="FN3" s="1" t="s">
+      <c r="FH3" s="17"/>
+      <c r="FJ3" s="4"/>
+      <c r="FN3" s="16"/>
+      <c r="FO3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="FQ3" s="1" t="s">
+      <c r="FR3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="FR3" s="1" t="s">
+      <c r="FS3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="FS3" s="1" t="s">
+      <c r="FT3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="FT3" s="1" t="s">
+      <c r="FU3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="FU3" s="1" t="s">
+      <c r="FV3" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="FV3" s="1" t="s">
+      <c r="FW3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="FX3" s="1">
+      <c r="FY3" s="1">
         <v>0</v>
       </c>
-      <c r="FY3" s="4" t="s">
+      <c r="FZ3" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="FZ3" s="1">
+      <c r="GA3" s="1">
         <v>100</v>
       </c>
-      <c r="GA3" s="1">
+      <c r="GB3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="GC3" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="GD3" s="1">
+        <v>15</v>
+      </c>
+      <c r="GE3" s="1">
         <v>0</v>
       </c>
-      <c r="GB3" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="GC3" s="1">
-        <v>15</v>
-      </c>
-      <c r="GD3" s="1">
-        <v>0</v>
-      </c>
-      <c r="GE3" s="4">
-        <v>1</v>
-      </c>
-      <c r="GF3" s="1">
+      <c r="GF3" s="4">
+        <v>1</v>
+      </c>
+      <c r="GG3" s="1">
         <v>6</v>
-      </c>
-      <c r="GG3" s="1">
-        <v>9</v>
       </c>
       <c r="GH3" s="1">
         <v>9</v>
       </c>
       <c r="GI3" s="1">
+        <v>9</v>
+      </c>
+      <c r="GJ3" s="1">
         <v>12</v>
       </c>
-      <c r="GJ3" s="1">
+      <c r="GK3" s="1">
         <v>2</v>
       </c>
-      <c r="GK3" s="1">
+      <c r="GL3" s="1">
         <v>25</v>
       </c>
-      <c r="GL3" s="1">
+      <c r="GM3" s="1">
         <v>0</v>
       </c>
-      <c r="GM3" s="9"/>
-      <c r="GN3" s="1" t="s">
+      <c r="GN3" s="9"/>
+      <c r="GO3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="GO3" s="1" t="s">
+      <c r="GP3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="GP3" s="1" t="s">
+      <c r="GQ3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="GQ3" s="1" t="s">
+      <c r="GR3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="GU3" s="4"/>
-      <c r="GX3" s="4"/>
-      <c r="GZ3" s="4"/>
-      <c r="HC3" s="22"/>
-      <c r="HD3" s="11" t="s">
+      <c r="GV3" s="4"/>
+      <c r="GY3" s="4"/>
+      <c r="HA3" s="4"/>
+      <c r="HD3" s="22"/>
+      <c r="HE3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="HE3" s="11" t="s">
+      <c r="HF3" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="HF3" s="11" t="s">
+      <c r="HG3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="HG3" s="11" t="s">
+      <c r="HH3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="HH3" s="11" t="s">
+      <c r="HI3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="HI3" s="11" t="s">
+      <c r="HJ3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="HJ3" s="11"/>
       <c r="HK3" s="11"/>
-      <c r="HL3" s="11">
+      <c r="HL3" s="11"/>
+      <c r="HM3" s="11">
         <v>80</v>
       </c>
-      <c r="HM3" s="11">
+      <c r="HN3" s="11">
         <v>800</v>
       </c>
-      <c r="HN3" s="11">
+      <c r="HO3" s="11">
         <v>90</v>
       </c>
-      <c r="HO3" s="11">
-        <v>1</v>
-      </c>
-      <c r="HP3" s="12" t="s">
+      <c r="HP3" s="11">
+        <v>1</v>
+      </c>
+      <c r="HQ3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="HQ3" s="12" t="s">
+      <c r="HR3" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="HR3" s="11">
+      <c r="HS3" s="11">
         <v>89</v>
       </c>
-      <c r="HS3" s="12">
+      <c r="HT3" s="12">
         <v>12</v>
       </c>
-      <c r="HT3" s="12">
+      <c r="HU3" s="12">
         <v>0</v>
       </c>
-      <c r="HU3" s="12">
+      <c r="HV3" s="12">
         <v>0.02</v>
       </c>
-      <c r="HV3" s="11">
+      <c r="HW3" s="11">
         <v>0.09</v>
       </c>
-      <c r="HW3" s="11">
-        <v>1</v>
-      </c>
       <c r="HX3" s="11">
+        <v>1</v>
+      </c>
+      <c r="HY3" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="R4" s="8"/>
-      <c r="AS4" s="19"/>
-      <c r="BK4" s="19"/>
-      <c r="CB4" s="19"/>
-      <c r="CF4" s="10"/>
+    <row r="4" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="AT4" s="19"/>
+      <c r="BL4" s="19"/>
+      <c r="CC4" s="19"/>
       <c r="CG4" s="10"/>
       <c r="CH4" s="10"/>
       <c r="CI4" s="10"/>
       <c r="CJ4" s="10"/>
       <c r="CK4" s="10"/>
-      <c r="CN4" s="10"/>
+      <c r="CL4" s="10"/>
       <c r="CO4" s="10"/>
       <c r="CP4" s="10"/>
       <c r="CQ4" s="10"/>
       <c r="CR4" s="10"/>
-      <c r="CS4" s="13"/>
-      <c r="CT4" s="10"/>
+      <c r="CS4" s="10"/>
+      <c r="CT4" s="13"/>
       <c r="CU4" s="10"/>
       <c r="CV4" s="10"/>
       <c r="CW4" s="10"/>
-      <c r="DB4" s="10"/>
+      <c r="CX4" s="10"/>
       <c r="DC4" s="10"/>
       <c r="DD4" s="10"/>
       <c r="DE4" s="10"/>
       <c r="DF4" s="10"/>
       <c r="DG4" s="10"/>
-      <c r="DI4" s="10"/>
+      <c r="DH4" s="10"/>
       <c r="DJ4" s="10"/>
       <c r="DK4" s="10"/>
       <c r="DL4" s="10"/>
       <c r="DM4" s="10"/>
       <c r="DN4" s="10"/>
-      <c r="DO4" s="13"/>
-      <c r="DP4" s="10"/>
+      <c r="DO4" s="10"/>
+      <c r="DP4" s="13"/>
       <c r="DQ4" s="10"/>
       <c r="DR4" s="10"/>
       <c r="DS4" s="10"/>
-      <c r="DT4" s="14"/>
-      <c r="EF4" s="8"/>
-      <c r="EI4" s="8"/>
-      <c r="EL4" s="8"/>
-      <c r="ET4" s="14"/>
-      <c r="FM4" s="15"/>
-      <c r="FY4" s="8"/>
-      <c r="GB4" s="8"/>
-      <c r="GE4" s="8"/>
-      <c r="GM4" s="14"/>
-      <c r="HC4" s="21"/>
+      <c r="DT4" s="10"/>
+      <c r="DU4" s="14"/>
+      <c r="EG4" s="8"/>
+      <c r="EJ4" s="8"/>
+      <c r="EM4" s="8"/>
+      <c r="EU4" s="14"/>
+      <c r="FN4" s="15"/>
+      <c r="FZ4" s="8"/>
+      <c r="GC4" s="8"/>
+      <c r="GF4" s="8"/>
+      <c r="GN4" s="14"/>
+      <c r="HD4" s="21"/>
     </row>
-    <row r="5" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="R5" s="8"/>
-      <c r="AS5" s="19"/>
-      <c r="BK5" s="19"/>
-      <c r="CB5" s="19"/>
-      <c r="CS5" s="8"/>
-      <c r="DO5" s="8"/>
-      <c r="DT5" s="14"/>
-      <c r="EF5" s="8"/>
-      <c r="EI5" s="8"/>
-      <c r="EL5" s="8"/>
-      <c r="ET5" s="14"/>
-      <c r="FM5" s="15"/>
-      <c r="FY5" s="8"/>
-      <c r="GB5" s="8"/>
-      <c r="GE5" s="8"/>
-      <c r="GM5" s="14"/>
-      <c r="HC5" s="21"/>
+    <row r="5" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="AT5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="CC5" s="19"/>
+      <c r="CT5" s="8"/>
+      <c r="DP5" s="8"/>
+      <c r="DU5" s="14"/>
+      <c r="EG5" s="8"/>
+      <c r="EJ5" s="8"/>
+      <c r="EM5" s="8"/>
+      <c r="EU5" s="14"/>
+      <c r="FN5" s="15"/>
+      <c r="FZ5" s="8"/>
+      <c r="GC5" s="8"/>
+      <c r="GF5" s="8"/>
+      <c r="GN5" s="14"/>
+      <c r="HD5" s="21"/>
     </row>
-    <row r="6" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="AS6" s="19"/>
-      <c r="BK6" s="19"/>
-      <c r="CB6" s="19"/>
-      <c r="CS6" s="8"/>
-      <c r="DO6" s="8"/>
-      <c r="DT6" s="14"/>
-      <c r="EF6" s="8"/>
-      <c r="EI6" s="8"/>
-      <c r="EL6" s="8"/>
-      <c r="ET6" s="14"/>
-      <c r="FM6" s="15"/>
-      <c r="FY6" s="8"/>
-      <c r="GB6" s="8"/>
-      <c r="GE6" s="8"/>
-      <c r="GM6" s="14"/>
-      <c r="HC6" s="21"/>
+    <row r="6" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="AT6" s="19"/>
+      <c r="BL6" s="19"/>
+      <c r="CC6" s="19"/>
+      <c r="CT6" s="8"/>
+      <c r="DP6" s="8"/>
+      <c r="DU6" s="14"/>
+      <c r="EG6" s="8"/>
+      <c r="EJ6" s="8"/>
+      <c r="EM6" s="8"/>
+      <c r="EU6" s="14"/>
+      <c r="FN6" s="15"/>
+      <c r="FZ6" s="8"/>
+      <c r="GC6" s="8"/>
+      <c r="GF6" s="8"/>
+      <c r="GN6" s="14"/>
+      <c r="HD6" s="21"/>
     </row>
-    <row r="7" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="R7" s="8"/>
-      <c r="AS7" s="19"/>
-      <c r="BK7" s="19"/>
-      <c r="CB7" s="19"/>
-      <c r="CS7" s="8"/>
-      <c r="DO7" s="8"/>
-      <c r="DT7" s="14"/>
-      <c r="EF7" s="8"/>
-      <c r="EI7" s="8"/>
-      <c r="EL7" s="8"/>
-      <c r="ET7" s="14"/>
-      <c r="FM7" s="15"/>
-      <c r="FY7" s="8"/>
-      <c r="GB7" s="8"/>
-      <c r="GE7" s="8"/>
-      <c r="GM7" s="14"/>
-      <c r="HC7" s="21"/>
+    <row r="7" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="8"/>
+      <c r="P7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="AT7" s="19"/>
+      <c r="BL7" s="19"/>
+      <c r="CC7" s="19"/>
+      <c r="CT7" s="8"/>
+      <c r="DP7" s="8"/>
+      <c r="DU7" s="14"/>
+      <c r="EG7" s="8"/>
+      <c r="EJ7" s="8"/>
+      <c r="EM7" s="8"/>
+      <c r="EU7" s="14"/>
+      <c r="FN7" s="15"/>
+      <c r="FZ7" s="8"/>
+      <c r="GC7" s="8"/>
+      <c r="GF7" s="8"/>
+      <c r="GN7" s="14"/>
+      <c r="HD7" s="21"/>
     </row>
-    <row r="8" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="AS8" s="19"/>
-      <c r="BK8" s="19"/>
-      <c r="CB8" s="19"/>
-      <c r="CS8" s="8"/>
-      <c r="DO8" s="8"/>
-      <c r="DT8" s="14"/>
-      <c r="EF8" s="8"/>
-      <c r="EI8" s="8"/>
-      <c r="EL8" s="8"/>
-      <c r="ET8" s="14"/>
-      <c r="FM8" s="15"/>
-      <c r="FY8" s="8"/>
-      <c r="GB8" s="8"/>
-      <c r="GE8" s="8"/>
-      <c r="GM8" s="14"/>
-      <c r="HC8" s="21"/>
+    <row r="8" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="S8" s="8"/>
+      <c r="AT8" s="19"/>
+      <c r="BL8" s="19"/>
+      <c r="CC8" s="19"/>
+      <c r="CT8" s="8"/>
+      <c r="DP8" s="8"/>
+      <c r="DU8" s="14"/>
+      <c r="EG8" s="8"/>
+      <c r="EJ8" s="8"/>
+      <c r="EM8" s="8"/>
+      <c r="EU8" s="14"/>
+      <c r="FN8" s="15"/>
+      <c r="FZ8" s="8"/>
+      <c r="GC8" s="8"/>
+      <c r="GF8" s="8"/>
+      <c r="GN8" s="14"/>
+      <c r="HD8" s="21"/>
     </row>
-    <row r="9" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="R9" s="8"/>
-      <c r="AS9" s="19"/>
-      <c r="BK9" s="19"/>
-      <c r="CB9" s="19"/>
-      <c r="CS9" s="8"/>
-      <c r="DO9" s="8"/>
-      <c r="DT9" s="14"/>
-      <c r="EF9" s="8"/>
-      <c r="EI9" s="8"/>
-      <c r="EL9" s="8"/>
-      <c r="ET9" s="14"/>
-      <c r="FM9" s="15"/>
-      <c r="FY9" s="8"/>
-      <c r="GB9" s="8"/>
-      <c r="GE9" s="8"/>
-      <c r="GM9" s="14"/>
-      <c r="HC9" s="21"/>
+    <row r="9" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M9" s="8"/>
+      <c r="P9" s="8"/>
+      <c r="S9" s="8"/>
+      <c r="AT9" s="19"/>
+      <c r="BL9" s="19"/>
+      <c r="CC9" s="19"/>
+      <c r="CT9" s="8"/>
+      <c r="DP9" s="8"/>
+      <c r="DU9" s="14"/>
+      <c r="EG9" s="8"/>
+      <c r="EJ9" s="8"/>
+      <c r="EM9" s="8"/>
+      <c r="EU9" s="14"/>
+      <c r="FN9" s="15"/>
+      <c r="FZ9" s="8"/>
+      <c r="GC9" s="8"/>
+      <c r="GF9" s="8"/>
+      <c r="GN9" s="14"/>
+      <c r="HD9" s="21"/>
     </row>
-    <row r="10" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="AS10" s="19"/>
-      <c r="BK10" s="19"/>
-      <c r="CB10" s="19"/>
-      <c r="CS10" s="8"/>
-      <c r="DO10" s="8"/>
-      <c r="DT10" s="14"/>
-      <c r="EF10" s="8"/>
-      <c r="EI10" s="8"/>
-      <c r="EL10" s="8"/>
-      <c r="ET10" s="14"/>
-      <c r="FM10" s="15"/>
-      <c r="FY10" s="8"/>
-      <c r="GB10" s="8"/>
-      <c r="GE10" s="8"/>
-      <c r="GM10" s="14"/>
-      <c r="HC10" s="21"/>
+    <row r="10" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M10" s="8"/>
+      <c r="P10" s="8"/>
+      <c r="S10" s="8"/>
+      <c r="AT10" s="19"/>
+      <c r="BL10" s="19"/>
+      <c r="CC10" s="19"/>
+      <c r="CT10" s="8"/>
+      <c r="DP10" s="8"/>
+      <c r="DU10" s="14"/>
+      <c r="EG10" s="8"/>
+      <c r="EJ10" s="8"/>
+      <c r="EM10" s="8"/>
+      <c r="EU10" s="14"/>
+      <c r="FN10" s="15"/>
+      <c r="FZ10" s="8"/>
+      <c r="GC10" s="8"/>
+      <c r="GF10" s="8"/>
+      <c r="GN10" s="14"/>
+      <c r="HD10" s="21"/>
     </row>
-    <row r="11" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="AS11" s="19"/>
-      <c r="BK11" s="19"/>
-      <c r="CB11" s="19"/>
-      <c r="CS11" s="8"/>
-      <c r="DO11" s="8"/>
-      <c r="DT11" s="14"/>
-      <c r="EF11" s="8"/>
-      <c r="EI11" s="8"/>
-      <c r="EL11" s="8"/>
-      <c r="ET11" s="14"/>
-      <c r="FM11" s="15"/>
-      <c r="FY11" s="8"/>
-      <c r="GB11" s="8"/>
-      <c r="GE11" s="8"/>
-      <c r="GM11" s="14"/>
-      <c r="HC11" s="21"/>
+    <row r="11" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="AT11" s="19"/>
+      <c r="BL11" s="19"/>
+      <c r="CC11" s="19"/>
+      <c r="CT11" s="8"/>
+      <c r="DP11" s="8"/>
+      <c r="DU11" s="14"/>
+      <c r="EG11" s="8"/>
+      <c r="EJ11" s="8"/>
+      <c r="EM11" s="8"/>
+      <c r="EU11" s="14"/>
+      <c r="FN11" s="15"/>
+      <c r="FZ11" s="8"/>
+      <c r="GC11" s="8"/>
+      <c r="GF11" s="8"/>
+      <c r="GN11" s="14"/>
+      <c r="HD11" s="21"/>
     </row>
-    <row r="12" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="AS12" s="19"/>
-      <c r="BK12" s="19"/>
-      <c r="CB12" s="19"/>
-      <c r="CS12" s="8"/>
-      <c r="DO12" s="8"/>
-      <c r="DT12" s="14"/>
-      <c r="EF12" s="8"/>
-      <c r="EI12" s="8"/>
-      <c r="EL12" s="8"/>
-      <c r="ET12" s="14"/>
-      <c r="FM12" s="15"/>
-      <c r="FY12" s="8"/>
-      <c r="GB12" s="8"/>
-      <c r="GE12" s="8"/>
-      <c r="GM12" s="14"/>
-      <c r="HC12" s="21"/>
+    <row r="12" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="AT12" s="19"/>
+      <c r="BL12" s="19"/>
+      <c r="CC12" s="19"/>
+      <c r="CT12" s="8"/>
+      <c r="DP12" s="8"/>
+      <c r="DU12" s="14"/>
+      <c r="EG12" s="8"/>
+      <c r="EJ12" s="8"/>
+      <c r="EM12" s="8"/>
+      <c r="EU12" s="14"/>
+      <c r="FN12" s="15"/>
+      <c r="FZ12" s="8"/>
+      <c r="GC12" s="8"/>
+      <c r="GF12" s="8"/>
+      <c r="GN12" s="14"/>
+      <c r="HD12" s="21"/>
     </row>
-    <row r="13" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="AS13" s="19"/>
-      <c r="BK13" s="19"/>
-      <c r="CB13" s="19"/>
-      <c r="CS13" s="8"/>
-      <c r="DO13" s="8"/>
-      <c r="DT13" s="14"/>
-      <c r="EF13" s="8"/>
-      <c r="EI13" s="8"/>
-      <c r="EL13" s="8"/>
-      <c r="ET13" s="14"/>
-      <c r="FM13" s="15"/>
-      <c r="FY13" s="8"/>
-      <c r="GB13" s="8"/>
-      <c r="GE13" s="8"/>
-      <c r="GM13" s="14"/>
-      <c r="HC13" s="21"/>
+    <row r="13" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="AT13" s="19"/>
+      <c r="BL13" s="19"/>
+      <c r="CC13" s="19"/>
+      <c r="CT13" s="8"/>
+      <c r="DP13" s="8"/>
+      <c r="DU13" s="14"/>
+      <c r="EG13" s="8"/>
+      <c r="EJ13" s="8"/>
+      <c r="EM13" s="8"/>
+      <c r="EU13" s="14"/>
+      <c r="FN13" s="15"/>
+      <c r="FZ13" s="8"/>
+      <c r="GC13" s="8"/>
+      <c r="GF13" s="8"/>
+      <c r="GN13" s="14"/>
+      <c r="HD13" s="21"/>
     </row>
-    <row r="14" spans="1:232" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="L14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="AS14" s="19"/>
-      <c r="BK14" s="19"/>
-      <c r="CB14" s="19"/>
-      <c r="CM14"/>
-      <c r="CS14" s="8"/>
-      <c r="DI14"/>
-      <c r="DO14" s="8"/>
-      <c r="DT14" s="14"/>
-      <c r="EF14" s="8"/>
-      <c r="EI14" s="8"/>
-      <c r="EL14" s="8"/>
-      <c r="ET14" s="14"/>
-      <c r="FM14" s="15"/>
-      <c r="FY14" s="8"/>
-      <c r="GB14" s="8"/>
-      <c r="GE14" s="8"/>
-      <c r="GM14" s="14"/>
-      <c r="HC14" s="21"/>
+    <row r="14" spans="1:233" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="M14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="AT14" s="19"/>
+      <c r="BL14" s="19"/>
+      <c r="CC14" s="19"/>
+      <c r="CN14"/>
+      <c r="CT14" s="8"/>
+      <c r="DJ14"/>
+      <c r="DP14" s="8"/>
+      <c r="DU14" s="14"/>
+      <c r="EG14" s="8"/>
+      <c r="EJ14" s="8"/>
+      <c r="EM14" s="8"/>
+      <c r="EU14" s="14"/>
+      <c r="FN14" s="15"/>
+      <c r="FZ14" s="8"/>
+      <c r="GC14" s="8"/>
+      <c r="GF14" s="8"/>
+      <c r="GN14" s="14"/>
+      <c r="HD14" s="21"/>
     </row>
-    <row r="15" spans="1:232" x14ac:dyDescent="0.2">
-      <c r="CC15" s="7"/>
+    <row r="15" spans="1:233" x14ac:dyDescent="0.2">
       <c r="CD15" s="7"/>
       <c r="CE15" s="7"/>
       <c r="CF15" s="7"/>
@@ -3078,17 +3089,17 @@
       <c r="CI15" s="7"/>
       <c r="CJ15" s="7"/>
       <c r="CK15" s="7"/>
-      <c r="CN15" s="7"/>
+      <c r="CL15" s="7"/>
       <c r="CO15" s="7"/>
       <c r="CP15" s="7"/>
       <c r="CQ15" s="7"/>
       <c r="CR15" s="7"/>
-      <c r="CS15" s="8"/>
-      <c r="CT15" s="7"/>
+      <c r="CS15" s="7"/>
+      <c r="CT15" s="8"/>
       <c r="CU15" s="7"/>
       <c r="CV15" s="7"/>
       <c r="CW15" s="7"/>
-      <c r="CY15" s="7"/>
+      <c r="CX15" s="7"/>
       <c r="CZ15" s="7"/>
       <c r="DA15" s="7"/>
       <c r="DB15" s="7"/>
@@ -3097,16 +3108,17 @@
       <c r="DE15" s="7"/>
       <c r="DF15" s="7"/>
       <c r="DG15" s="7"/>
-      <c r="DJ15" s="7"/>
+      <c r="DH15" s="7"/>
       <c r="DK15" s="7"/>
       <c r="DL15" s="7"/>
       <c r="DM15" s="7"/>
       <c r="DN15" s="7"/>
-      <c r="DO15" s="8"/>
-      <c r="DP15" s="7"/>
+      <c r="DO15" s="7"/>
+      <c r="DP15" s="8"/>
       <c r="DQ15" s="7"/>
       <c r="DR15" s="7"/>
       <c r="DS15" s="7"/>
+      <c r="DT15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>